<commit_message>
actualizo info de Estonia al 2015
</commit_message>
<xml_diff>
--- a/doc/memoria/recursos/estonia.xlsx
+++ b/doc/memoria/recursos/estonia.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="130" uniqueCount="86">
   <si>
     <t>Local elections</t>
   </si>
@@ -309,6 +309,15 @@
   </si>
   <si>
     <t>Fuente:</t>
+  </si>
+  <si>
+    <t>2105 Parl</t>
+  </si>
+  <si>
+    <t>116 states</t>
+  </si>
+  <si>
+    <t>22 084</t>
   </si>
 </sst>
 </file>
@@ -592,7 +601,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
@@ -672,6 +681,25 @@
     <xf numFmtId="10" fontId="2" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -690,29 +718,19 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -751,9 +769,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja2!$B$1:$H$1</c:f>
+              <c:f>Hoja2!$B$1:$I$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>2005 Local</c:v>
                 </c:pt>
@@ -774,16 +792,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2014 EU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2105 Parl</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja2!$B$2:$H$2</c:f>
+              <c:f>Hoja2!$B$2:$I$2</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1059292</c:v>
                 </c:pt>
@@ -804,6 +825,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>902873</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>899793</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -857,10 +881,10 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja2!$B$3:$H$3</c:f>
+              <c:f>Hoja2!$B$3:$I$3</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>502504</c:v>
                 </c:pt>
@@ -881,6 +905,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>329766</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>577910</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -905,10 +932,10 @@
           </c:marker>
           <c:val>
             <c:numRef>
-              <c:f>Hoja2!$B$5:$H$5</c:f>
+              <c:f>Hoja2!$B$5:$I$5</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>9317</c:v>
                 </c:pt>
@@ -929,30 +956,33 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>103151</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>176491</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="51801472"/>
-        <c:axId val="52163712"/>
+        <c:axId val="69483136"/>
+        <c:axId val="69497216"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="51801472"/>
+        <c:axId val="69483136"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="52163712"/>
+        <c:crossAx val="69497216"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="52163712"/>
+        <c:axId val="69497216"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -960,7 +990,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="51801472"/>
+        <c:crossAx val="69483136"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -973,7 +1003,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageMargins b="0.75000000000000011" l="0.70000000000000007" r="0.70000000000000007" t="0.75000000000000011" header="0.30000000000000004" footer="0.30000000000000004"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1009,9 +1039,9 @@
           </c:marker>
           <c:cat>
             <c:strRef>
-              <c:f>Hoja2!$B$1:$H$1</c:f>
+              <c:f>Hoja2!$B$1:$I$1</c:f>
               <c:strCache>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>2005 Local</c:v>
                 </c:pt>
@@ -1032,16 +1062,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>2014 EU</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>2105 Parl</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Hoja2!$B$12:$H$12</c:f>
+              <c:f>Hoja2!$B$12:$I$12</c:f>
               <c:numCache>
                 <c:formatCode>0.00%</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>1.9E-2</c:v>
                 </c:pt>
@@ -1062,30 +1095,33 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>0.313</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.30499999999999999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
         </c:ser>
         <c:marker val="1"/>
-        <c:axId val="95748480"/>
-        <c:axId val="95750016"/>
+        <c:axId val="69504384"/>
+        <c:axId val="69518464"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="95748480"/>
+        <c:axId val="69504384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:axPos val="b"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95750016"/>
+        <c:crossAx val="69518464"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="95750016"/>
+        <c:axId val="69518464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1093,7 +1129,7 @@
         <c:majorGridlines/>
         <c:numFmt formatCode="0.00%" sourceLinked="1"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="95748480"/>
+        <c:crossAx val="69504384"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1106,7 +1142,7 @@
   </c:chart>
   <c:printSettings>
     <c:headerFooter/>
-    <c:pageMargins b="0.75000000000000022" l="0.70000000000000018" r="0.70000000000000018" t="0.75000000000000022" header="0.3000000000000001" footer="0.3000000000000001"/>
+    <c:pageMargins b="0.75000000000000033" l="0.70000000000000029" r="0.70000000000000029" t="0.75000000000000033" header="0.30000000000000016" footer="0.30000000000000016"/>
     <c:pageSetup/>
   </c:printSettings>
 </c:chartSpace>
@@ -1116,13 +1152,13 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
       <xdr:row>1</xdr:row>
       <xdr:rowOff>276225</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>447675</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>419100</xdr:rowOff>
@@ -1146,13 +1182,13 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
+      <xdr:col>9</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>457200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>14</xdr:col>
+      <xdr:col>15</xdr:col>
       <xdr:colOff>428625</xdr:colOff>
       <xdr:row>12</xdr:row>
       <xdr:rowOff>371475</xdr:rowOff>
@@ -1462,16 +1498,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:Q21"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="I22" sqref="I22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:15" ht="24.75">
-      <c r="A1" s="27"/>
+    <row r="1" spans="1:17" ht="24.75">
+      <c r="A1" s="34"/>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
@@ -1490,12 +1526,15 @@
       <c r="G1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="H1" s="30" t="s">
+      <c r="H1" s="37" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:15">
-      <c r="A2" s="28"/>
+      <c r="I1" s="2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17">
+      <c r="A2" s="35"/>
       <c r="B2" s="3">
         <v>2005</v>
       </c>
@@ -1514,10 +1553,13 @@
       <c r="G2" s="3">
         <v>2013</v>
       </c>
-      <c r="H2" s="31"/>
-    </row>
-    <row r="3" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A3" s="29"/>
+      <c r="H2" s="38"/>
+      <c r="I2" s="44">
+        <v>2015</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A3" s="36"/>
       <c r="B3" s="4"/>
       <c r="C3" s="4"/>
       <c r="D3" s="5">
@@ -1526,9 +1568,10 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
       <c r="G3" s="4"/>
-      <c r="H3" s="32"/>
-    </row>
-    <row r="4" spans="1:15" ht="25.5" thickBot="1">
+      <c r="H3" s="39"/>
+      <c r="I3" s="44"/>
+    </row>
+    <row r="4" spans="1:17" ht="25.5" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>5</v>
       </c>
@@ -1553,36 +1596,43 @@
       <c r="H4" s="17" t="s">
         <v>12</v>
       </c>
-      <c r="I4">
+      <c r="I4" s="7">
+        <v>899793</v>
+      </c>
+      <c r="J4">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B4, " ","")," ",""))</f>
         <v>1059292</v>
       </c>
-      <c r="J4">
-        <f t="shared" ref="J4:O4" si="0">VALUE(SUBSTITUTE(SUBSTITUTE(C4, " ","")," ",""))</f>
+      <c r="K4">
+        <f t="shared" ref="K4:Q4" si="0">VALUE(SUBSTITUTE(SUBSTITUTE(C4, " ","")," ",""))</f>
         <v>897243</v>
       </c>
-      <c r="K4">
+      <c r="L4">
         <f t="shared" si="0"/>
         <v>909628</v>
       </c>
-      <c r="L4">
+      <c r="M4">
         <f t="shared" si="0"/>
         <v>1094317</v>
       </c>
-      <c r="M4">
+      <c r="N4">
         <f t="shared" si="0"/>
         <v>913346</v>
       </c>
-      <c r="N4">
+      <c r="O4">
         <f t="shared" si="0"/>
         <v>1086935</v>
       </c>
-      <c r="O4">
+      <c r="P4">
         <f t="shared" si="0"/>
         <v>902873</v>
       </c>
-    </row>
-    <row r="5" spans="1:15" ht="37.5" thickBot="1">
+      <c r="Q4">
+        <f t="shared" si="0"/>
+        <v>899793</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" ht="37.5" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>13</v>
       </c>
@@ -1607,36 +1657,43 @@
       <c r="H5" s="17" t="s">
         <v>20</v>
       </c>
-      <c r="I5">
-        <f t="shared" ref="I5:I21" si="1">VALUE(SUBSTITUTE(SUBSTITUTE(B5, " ","")," ",""))</f>
+      <c r="I5" s="7">
+        <v>577910</v>
+      </c>
+      <c r="J5">
+        <f t="shared" ref="J5:J21" si="1">VALUE(SUBSTITUTE(SUBSTITUTE(B5, " ","")," ",""))</f>
         <v>502504</v>
       </c>
-      <c r="J5">
-        <f t="shared" ref="J5:J21" si="2">VALUE(SUBSTITUTE(SUBSTITUTE(C5, " ","")," ",""))</f>
+      <c r="K5">
+        <f t="shared" ref="K5:K21" si="2">VALUE(SUBSTITUTE(SUBSTITUTE(C5, " ","")," ",""))</f>
         <v>555463</v>
       </c>
-      <c r="K5">
-        <f t="shared" ref="K5:K21" si="3">VALUE(SUBSTITUTE(SUBSTITUTE(D5, " ","")," ",""))</f>
+      <c r="L5">
+        <f t="shared" ref="L5:L21" si="3">VALUE(SUBSTITUTE(SUBSTITUTE(D5, " ","")," ",""))</f>
         <v>399181</v>
       </c>
-      <c r="L5">
-        <f t="shared" ref="L5:L21" si="4">VALUE(SUBSTITUTE(SUBSTITUTE(E5, " ","")," ",""))</f>
+      <c r="M5">
+        <f t="shared" ref="M5:M21" si="4">VALUE(SUBSTITUTE(SUBSTITUTE(E5, " ","")," ",""))</f>
         <v>662813</v>
       </c>
-      <c r="M5">
-        <f t="shared" ref="M5:M21" si="5">VALUE(SUBSTITUTE(SUBSTITUTE(F5, " ","")," ",""))</f>
+      <c r="N5">
+        <f t="shared" ref="N5:N21" si="5">VALUE(SUBSTITUTE(SUBSTITUTE(F5, " ","")," ",""))</f>
         <v>580264</v>
       </c>
-      <c r="N5">
-        <f t="shared" ref="N5:N21" si="6">VALUE(SUBSTITUTE(SUBSTITUTE(G5, " ","")," ",""))</f>
+      <c r="O5">
+        <f t="shared" ref="O5:O19" si="6">VALUE(SUBSTITUTE(SUBSTITUTE(G5, " ","")," ",""))</f>
         <v>630050</v>
       </c>
-      <c r="O5">
-        <f t="shared" ref="O5:O21" si="7">VALUE(SUBSTITUTE(SUBSTITUTE(H5, " ","")," ",""))</f>
+      <c r="P5">
+        <f t="shared" ref="P5:Q19" si="7">VALUE(SUBSTITUTE(SUBSTITUTE(H5, " ","")," ",""))</f>
         <v>329766</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="25.5" thickBot="1">
+      <c r="Q5">
+        <f t="shared" si="7"/>
+        <v>577910</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" ht="25.5" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>21</v>
       </c>
@@ -1661,36 +1718,43 @@
       <c r="H6" s="18">
         <v>0.36499999999999999</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="8">
+        <v>0.64200000000000002</v>
+      </c>
+      <c r="J6">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B6, "%","")," ",""))</f>
         <v>0.47399999999999998</v>
       </c>
-      <c r="J6">
-        <f t="shared" ref="J6:O6" si="8">VALUE(SUBSTITUTE(SUBSTITUTE(C6, "%","")," ",""))</f>
+      <c r="K6">
+        <f t="shared" ref="K6:Q6" si="8">VALUE(SUBSTITUTE(SUBSTITUTE(C6, "%","")," ",""))</f>
         <v>0.61899999999999999</v>
       </c>
-      <c r="K6">
+      <c r="L6">
         <f t="shared" si="8"/>
         <v>0.439</v>
       </c>
-      <c r="L6">
+      <c r="M6">
         <f t="shared" si="8"/>
         <v>0.60599999999999998</v>
       </c>
-      <c r="M6">
+      <c r="N6">
         <f t="shared" si="8"/>
         <v>0.63500000000000001</v>
       </c>
-      <c r="N6">
+      <c r="O6">
         <f t="shared" si="8"/>
         <v>0.57999999999999996</v>
       </c>
-      <c r="O6">
+      <c r="P6">
         <f t="shared" si="8"/>
         <v>0.36499999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:15" ht="15.75" thickBot="1">
+      <c r="Q6">
+        <f t="shared" si="8"/>
+        <v>0.64200000000000002</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" ht="15.75" thickBot="1">
       <c r="A7" s="6" t="s">
         <v>22</v>
       </c>
@@ -1715,36 +1779,43 @@
       <c r="H7" s="17" t="s">
         <v>29</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="7">
+        <v>176491</v>
+      </c>
+      <c r="J7">
         <f t="shared" si="1"/>
         <v>9317</v>
       </c>
-      <c r="J7">
+      <c r="K7">
         <f t="shared" si="2"/>
         <v>30275</v>
       </c>
-      <c r="K7">
+      <c r="L7">
         <f t="shared" si="3"/>
         <v>58669</v>
       </c>
-      <c r="L7">
+      <c r="M7">
         <f t="shared" si="4"/>
         <v>104413</v>
       </c>
-      <c r="M7">
+      <c r="N7">
         <f t="shared" si="5"/>
         <v>140846</v>
       </c>
-      <c r="N7">
+      <c r="O7">
         <f t="shared" si="6"/>
         <v>133808</v>
       </c>
-      <c r="O7">
+      <c r="P7">
         <f t="shared" si="7"/>
         <v>103151</v>
       </c>
-    </row>
-    <row r="8" spans="1:15" ht="25.5" thickBot="1">
+      <c r="Q7">
+        <f t="shared" si="7"/>
+        <v>176491</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" ht="25.5" thickBot="1">
       <c r="A8" s="6" t="s">
         <v>30</v>
       </c>
@@ -1769,130 +1840,149 @@
       <c r="H8" s="19" t="s">
         <v>37</v>
       </c>
-      <c r="I8">
+      <c r="I8" s="7">
+        <v>176329</v>
+      </c>
+      <c r="J8">
         <f t="shared" si="1"/>
         <v>9287</v>
       </c>
-      <c r="J8">
+      <c r="K8">
         <f t="shared" si="2"/>
         <v>30243</v>
       </c>
-      <c r="K8">
+      <c r="L8">
         <f t="shared" si="3"/>
         <v>58614</v>
       </c>
-      <c r="L8">
+      <c r="M8">
         <f t="shared" si="4"/>
         <v>104313</v>
       </c>
-      <c r="M8">
+      <c r="N8">
         <f t="shared" si="5"/>
         <v>140764</v>
       </c>
-      <c r="N8">
+      <c r="O8">
         <f t="shared" si="6"/>
         <v>133662</v>
       </c>
-      <c r="O8">
+      <c r="P8">
         <f t="shared" si="7"/>
         <v>103105</v>
       </c>
-    </row>
-    <row r="9" spans="1:15" ht="24.75">
+      <c r="Q8">
+        <f t="shared" si="7"/>
+        <v>176329</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" ht="24.75">
       <c r="A9" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B9" s="33">
+      <c r="B9" s="32">
         <v>30</v>
       </c>
-      <c r="C9" s="33">
+      <c r="C9" s="32">
         <v>32</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="32">
         <v>55</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="32">
         <v>100</v>
       </c>
-      <c r="F9" s="33">
+      <c r="F9" s="32">
         <v>82</v>
       </c>
-      <c r="G9" s="33" t="s">
+      <c r="G9" s="32" t="s">
         <v>40</v>
       </c>
-      <c r="H9" s="35">
+      <c r="H9" s="40">
         <v>46</v>
       </c>
-      <c r="I9">
+      <c r="I9" s="32">
+        <v>162</v>
+      </c>
+      <c r="J9">
         <f t="shared" si="1"/>
         <v>30</v>
       </c>
-      <c r="J9">
+      <c r="K9">
         <f t="shared" si="2"/>
         <v>32</v>
       </c>
-      <c r="K9">
+      <c r="L9">
         <f t="shared" si="3"/>
         <v>55</v>
       </c>
-      <c r="L9">
+      <c r="M9">
         <f t="shared" si="4"/>
         <v>100</v>
       </c>
-      <c r="M9">
+      <c r="N9">
         <f t="shared" si="5"/>
         <v>82</v>
       </c>
-      <c r="N9">
+      <c r="O9">
         <f t="shared" si="6"/>
         <v>146</v>
       </c>
-      <c r="O9">
+      <c r="P9">
         <f t="shared" si="7"/>
         <v>46</v>
       </c>
-    </row>
-    <row r="10" spans="1:15" ht="37.5" thickBot="1">
+      <c r="Q9">
+        <f t="shared" si="7"/>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" ht="37.5" thickBot="1">
       <c r="A10" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="34"/>
-      <c r="C10" s="34"/>
-      <c r="D10" s="34"/>
-      <c r="E10" s="34"/>
-      <c r="F10" s="34"/>
-      <c r="G10" s="34"/>
-      <c r="H10" s="36"/>
-      <c r="I10" t="e">
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="41"/>
+      <c r="I10" s="33"/>
+      <c r="J10" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J10" t="e">
+      <c r="K10" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K10" t="e">
+      <c r="L10" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L10" t="e">
+      <c r="M10" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M10" t="e">
+      <c r="N10" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N10" t="e">
+      <c r="O10" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="O10" t="e">
+      <c r="P10" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="11" spans="1:15" ht="61.5" thickBot="1">
+      <c r="Q10" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" ht="61.5" thickBot="1">
       <c r="A11" s="6" t="s">
         <v>41</v>
       </c>
@@ -1917,36 +2007,43 @@
       <c r="H11" s="17" t="s">
         <v>42</v>
       </c>
-      <c r="I11" t="e">
+      <c r="I11" s="7">
+        <v>1</v>
+      </c>
+      <c r="J11" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J11" t="e">
+      <c r="K11" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K11" t="e">
+      <c r="L11" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L11" t="e">
+      <c r="M11" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M11" t="e">
+      <c r="N11" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N11">
+      <c r="O11">
         <f t="shared" si="6"/>
         <v>1</v>
       </c>
-      <c r="O11" t="e">
+      <c r="P11" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="12" spans="1:15" ht="49.5" thickBot="1">
+      <c r="Q11">
+        <f t="shared" si="7"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" ht="49.5" thickBot="1">
       <c r="A12" s="6" t="s">
         <v>44</v>
       </c>
@@ -1971,36 +2068,43 @@
       <c r="H12" s="17" t="s">
         <v>48</v>
       </c>
-      <c r="I12">
+      <c r="I12" s="7">
+        <v>4593</v>
+      </c>
+      <c r="J12">
         <f t="shared" si="1"/>
         <v>364</v>
       </c>
-      <c r="J12">
+      <c r="K12">
         <f t="shared" si="2"/>
         <v>789</v>
       </c>
-      <c r="K12">
+      <c r="L12">
         <f t="shared" si="3"/>
         <v>910</v>
       </c>
-      <c r="L12">
+      <c r="M12">
         <f t="shared" si="4"/>
         <v>2373</v>
       </c>
-      <c r="M12">
+      <c r="N12">
         <f t="shared" si="5"/>
         <v>4384</v>
       </c>
-      <c r="N12">
+      <c r="O12">
         <f t="shared" si="6"/>
         <v>3045</v>
       </c>
-      <c r="O12">
+      <c r="P12">
         <f t="shared" si="7"/>
         <v>2019</v>
       </c>
-    </row>
-    <row r="13" spans="1:15" ht="49.5" thickBot="1">
+      <c r="Q12">
+        <f t="shared" si="7"/>
+        <v>4593</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" ht="49.5" thickBot="1">
       <c r="A13" s="6" t="s">
         <v>49</v>
       </c>
@@ -2025,36 +2129,43 @@
       <c r="H13" s="18">
         <v>0.114</v>
       </c>
-      <c r="I13">
+      <c r="I13" s="8">
+        <v>0.19600000000000001</v>
+      </c>
+      <c r="J13">
         <f t="shared" si="1"/>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="J13">
+      <c r="K13">
         <f t="shared" si="2"/>
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="K13">
+      <c r="L13">
         <f t="shared" si="3"/>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="L13">
+      <c r="M13">
         <f t="shared" si="4"/>
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="M13">
+      <c r="N13">
         <f t="shared" si="5"/>
         <v>0.154</v>
       </c>
-      <c r="N13">
+      <c r="O13">
         <f t="shared" si="6"/>
         <v>0.123</v>
       </c>
-      <c r="O13">
+      <c r="P13">
         <f t="shared" si="7"/>
         <v>0.114</v>
       </c>
-    </row>
-    <row r="14" spans="1:15" ht="49.5" thickBot="1">
+      <c r="Q13">
+        <f t="shared" si="7"/>
+        <v>0.19600000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" ht="49.5" thickBot="1">
       <c r="A14" s="6" t="s">
         <v>51</v>
       </c>
@@ -2079,36 +2190,43 @@
       <c r="H14" s="20">
         <v>0.313</v>
       </c>
-      <c r="I14">
+      <c r="I14" s="13">
+        <v>0.30499999999999999</v>
+      </c>
+      <c r="J14">
         <f>VALUE(SUBSTITUTE(SUBSTITUTE(B14, "%","")," ",""))</f>
         <v>1.9E-2</v>
       </c>
-      <c r="J14">
-        <f t="shared" ref="J14:O14" si="9">VALUE(SUBSTITUTE(SUBSTITUTE(C14, "%","")," ",""))</f>
+      <c r="K14">
+        <f t="shared" ref="K14:Q15" si="9">VALUE(SUBSTITUTE(SUBSTITUTE(C14, "%","")," ",""))</f>
         <v>5.5E-2</v>
       </c>
-      <c r="K14">
+      <c r="L14">
         <f t="shared" si="9"/>
         <v>0.14699999999999999</v>
       </c>
-      <c r="L14">
+      <c r="M14">
         <f t="shared" si="9"/>
         <v>0.158</v>
       </c>
-      <c r="M14">
+      <c r="N14">
         <f t="shared" si="9"/>
         <v>0.24299999999999999</v>
       </c>
-      <c r="N14">
+      <c r="O14">
         <f t="shared" si="9"/>
         <v>0.21199999999999999</v>
       </c>
-      <c r="O14">
+      <c r="P14">
         <f t="shared" si="9"/>
         <v>0.313</v>
       </c>
-    </row>
-    <row r="15" spans="1:15" ht="49.5" thickBot="1">
+      <c r="Q14">
+        <f t="shared" si="9"/>
+        <v>0.30499999999999999</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" ht="49.5" thickBot="1">
       <c r="A15" s="6" t="s">
         <v>52</v>
       </c>
@@ -2133,40 +2251,47 @@
       <c r="H15" s="18">
         <v>0.59199999999999997</v>
       </c>
-      <c r="I15">
-        <f t="shared" ref="I15:I16" si="10">VALUE(SUBSTITUTE(SUBSTITUTE(B15, "%","")," ",""))*100</f>
-        <v>7.1999999999999993</v>
+      <c r="I15" s="43">
+        <v>0.59599999999999997</v>
       </c>
       <c r="J15">
-        <f t="shared" ref="J15:J16" si="11">VALUE(SUBSTITUTE(SUBSTITUTE(C15, "%","")," ",""))*100</f>
-        <v>17.599999999999998</v>
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(B15, "%","")," ",""))</f>
+        <v>7.1999999999999995E-2</v>
       </c>
       <c r="K15">
-        <f t="shared" ref="K15:K16" si="12">VALUE(SUBSTITUTE(SUBSTITUTE(D15, "%","")," ",""))*100</f>
-        <v>45.4</v>
+        <f t="shared" si="9"/>
+        <v>0.17599999999999999</v>
       </c>
       <c r="L15">
-        <f t="shared" ref="L15:L16" si="13">VALUE(SUBSTITUTE(SUBSTITUTE(E15, "%","")," ",""))*100</f>
-        <v>44</v>
+        <f t="shared" si="9"/>
+        <v>0.45400000000000001</v>
       </c>
       <c r="M15">
-        <f t="shared" ref="M15:M16" si="14">VALUE(SUBSTITUTE(SUBSTITUTE(F15, "%","")," ",""))*100</f>
-        <v>56.399999999999991</v>
-      </c>
-      <c r="N15" t="e">
-        <f t="shared" ref="N15:N16" si="15">VALUE(SUBSTITUTE(SUBSTITUTE(G15, "%","")," ",""))*100</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="O15">
-        <f t="shared" ref="O15:O16" si="16">VALUE(SUBSTITUTE(SUBSTITUTE(H15, "%","")," ",""))*100</f>
-        <v>59.199999999999996</v>
-      </c>
-    </row>
-    <row r="16" spans="1:15" ht="56.25" customHeight="1">
-      <c r="A16" s="37" t="s">
+        <f t="shared" si="9"/>
+        <v>0.44</v>
+      </c>
+      <c r="N15">
+        <f t="shared" si="9"/>
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="O15" t="e">
+        <f t="shared" si="9"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P15">
+        <f t="shared" si="9"/>
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="Q15">
+        <f t="shared" si="9"/>
+        <v>0.59599999999999997</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" ht="56.25" customHeight="1">
+      <c r="A16" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B16" s="33" t="s">
+      <c r="B16" s="32" t="s">
         <v>42</v>
       </c>
       <c r="C16" s="12" t="s">
@@ -2187,38 +2312,45 @@
       <c r="H16" s="21">
         <v>4.6899999999999997E-2</v>
       </c>
-      <c r="I16" t="e">
-        <f t="shared" si="10"/>
-        <v>#VALUE!</v>
+      <c r="I16" s="43">
+        <v>5.7099999999999998E-2</v>
       </c>
       <c r="J16" t="e">
-        <f t="shared" si="11"/>
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(B16, "%","")," ",""))*100</f>
         <v>#VALUE!</v>
       </c>
       <c r="K16" t="e">
-        <f t="shared" si="12"/>
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(C16, "%","")," ",""))*100</f>
         <v>#VALUE!</v>
       </c>
       <c r="L16" t="e">
-        <f t="shared" si="13"/>
-        <v>#VALUE!</v>
-      </c>
-      <c r="M16">
-        <f t="shared" si="14"/>
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(D16, "%","")," ",""))*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="M16" t="e">
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(E16, "%","")," ",""))*100</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N16">
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(F16, "%","")," ",""))*100</f>
         <v>3.9</v>
       </c>
-      <c r="N16">
-        <f t="shared" si="15"/>
+      <c r="O16">
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(G16, "%","")," ",""))*100</f>
         <v>4.2</v>
       </c>
-      <c r="O16">
-        <f t="shared" si="16"/>
+      <c r="P16">
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(H16, "%","")," ",""))*100</f>
         <v>4.6899999999999995</v>
       </c>
-    </row>
-    <row r="17" spans="1:15" ht="15.75" thickBot="1">
-      <c r="A17" s="38"/>
-      <c r="B17" s="34"/>
+      <c r="Q16">
+        <f>VALUE(SUBSTITUTE(SUBSTITUTE(I16, "%","")," ",""))*100</f>
+        <v>5.71</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A17" s="31"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="15" t="s">
         <v>56</v>
       </c>
@@ -2237,36 +2369,43 @@
       <c r="H17" s="22" t="s">
         <v>63</v>
       </c>
-      <c r="I17" t="e">
+      <c r="I17" s="42" t="s">
+        <v>84</v>
+      </c>
+      <c r="J17" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J17" t="e">
+      <c r="K17" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K17" t="e">
+      <c r="L17" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L17" t="e">
+      <c r="M17" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M17" t="e">
+      <c r="N17" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N17" t="e">
+      <c r="O17" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="O17" t="e">
+      <c r="P17" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="18" spans="1:15" ht="25.5" thickBot="1">
+      <c r="Q17" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" ht="25.5" thickBot="1">
       <c r="A18" s="6" t="s">
         <v>64</v>
       </c>
@@ -2291,36 +2430,43 @@
       <c r="H18" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="I18" t="e">
+      <c r="I18" s="42" t="s">
+        <v>66</v>
+      </c>
+      <c r="J18" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J18" t="e">
+      <c r="K18" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K18" t="e">
+      <c r="L18" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L18" t="e">
+      <c r="M18" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M18" t="e">
+      <c r="N18" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N18" t="e">
+      <c r="O18" t="e">
         <f t="shared" si="6"/>
         <v>#VALUE!</v>
       </c>
-      <c r="O18" t="e">
+      <c r="P18" t="e">
         <f t="shared" si="7"/>
         <v>#VALUE!</v>
       </c>
-    </row>
-    <row r="19" spans="1:15" ht="37.5" thickBot="1">
+      <c r="Q18" t="e">
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" ht="37.5" thickBot="1">
       <c r="A19" s="6" t="s">
         <v>68</v>
       </c>
@@ -2345,36 +2491,43 @@
       <c r="H19" s="17" t="s">
         <v>71</v>
       </c>
-      <c r="I19" t="e">
+      <c r="I19" s="42" t="s">
+        <v>85</v>
+      </c>
+      <c r="J19" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J19" t="e">
+      <c r="K19" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K19" t="e">
+      <c r="L19" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L19" t="e">
+      <c r="M19" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M19">
+      <c r="N19">
         <f t="shared" si="5"/>
         <v>2690</v>
       </c>
-      <c r="N19">
+      <c r="O19">
         <f t="shared" si="6"/>
         <v>11753</v>
       </c>
-      <c r="O19">
+      <c r="P19">
         <f t="shared" si="7"/>
         <v>11609</v>
       </c>
-    </row>
-    <row r="20" spans="1:15" ht="49.5" thickBot="1">
+      <c r="Q19">
+        <f t="shared" si="7"/>
+        <v>22084</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" ht="49.5" thickBot="1">
       <c r="A20" s="6" t="s">
         <v>72</v>
       </c>
@@ -2399,36 +2552,43 @@
       <c r="H20" s="18">
         <v>0.11</v>
       </c>
-      <c r="I20" t="e">
+      <c r="I20" s="43">
+        <v>0.122</v>
+      </c>
+      <c r="J20" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J20" t="e">
+      <c r="K20" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K20" t="e">
+      <c r="L20" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L20" t="e">
+      <c r="M20" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M20">
-        <f t="shared" ref="M20:O21" si="17">VALUE(SUBSTITUTE(SUBSTITUTE(F20, "%","")," ",""))*100</f>
+      <c r="N20">
+        <f t="shared" ref="N20:Q21" si="10">VALUE(SUBSTITUTE(SUBSTITUTE(F20, "%","")," ",""))*100</f>
         <v>1.9</v>
       </c>
-      <c r="N20">
-        <f t="shared" ref="N20" si="18">VALUE(SUBSTITUTE(SUBSTITUTE(G20, "%","")," ",""))*100</f>
+      <c r="O20">
+        <f t="shared" ref="O20" si="11">VALUE(SUBSTITUTE(SUBSTITUTE(G20, "%","")," ",""))*100</f>
         <v>8.6</v>
       </c>
-      <c r="O20">
-        <f t="shared" ref="O20" si="19">VALUE(SUBSTITUTE(SUBSTITUTE(H20, "%","")," ",""))*100</f>
+      <c r="P20">
+        <f t="shared" ref="P20:Q20" si="12">VALUE(SUBSTITUTE(SUBSTITUTE(H20, "%","")," ",""))*100</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="21" spans="1:15" ht="60.75">
+      <c r="Q20">
+        <f t="shared" si="12"/>
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" ht="60.75">
       <c r="A21" s="23" t="s">
         <v>73</v>
       </c>
@@ -2453,37 +2613,45 @@
       <c r="H21" s="26">
         <v>0.04</v>
       </c>
-      <c r="I21" t="e">
+      <c r="I21" s="43">
+        <v>4.2999999999999997E-2</v>
+      </c>
+      <c r="J21" t="e">
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
-      <c r="J21" t="e">
+      <c r="K21" t="e">
         <f t="shared" si="2"/>
         <v>#VALUE!</v>
       </c>
-      <c r="K21" t="e">
+      <c r="L21" t="e">
         <f t="shared" si="3"/>
         <v>#VALUE!</v>
       </c>
-      <c r="L21" t="e">
+      <c r="M21" t="e">
         <f t="shared" si="4"/>
         <v>#VALUE!</v>
       </c>
-      <c r="M21" t="e">
+      <c r="N21" t="e">
         <f t="shared" si="5"/>
         <v>#VALUE!</v>
       </c>
-      <c r="N21">
-        <f t="shared" si="17"/>
+      <c r="O21">
+        <f t="shared" si="10"/>
         <v>3.4000000000000004</v>
       </c>
-      <c r="O21">
-        <f t="shared" si="17"/>
+      <c r="P21">
+        <f t="shared" si="10"/>
         <v>4</v>
       </c>
+      <c r="Q21">
+        <f t="shared" si="10"/>
+        <v>4.3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
+  <mergeCells count="12">
+    <mergeCell ref="I9:I10"/>
     <mergeCell ref="A16:A17"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="A1:A3"/>
@@ -2503,15 +2671,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:J19"/>
+  <dimension ref="A1:K19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="Q9" sqref="Q9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:10">
+    <row r="1" spans="1:11">
       <c r="A1" s="1"/>
       <c r="B1" s="2" t="s">
         <v>75</v>
@@ -2531,568 +2699,646 @@
       <c r="G1" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="H1" s="39" t="s">
+      <c r="H1" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="I1" s="41" t="s">
+      <c r="I1" s="27" t="s">
+        <v>83</v>
+      </c>
+      <c r="J1" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="J1" s="40" t="s">
+      <c r="K1" s="28" t="s">
         <v>81</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="25.5" thickBot="1">
+    <row r="2" spans="1:11" ht="25.5" thickBot="1">
       <c r="A2" s="6" t="s">
         <v>5</v>
       </c>
       <c r="B2" s="7">
-        <f>Hoja1!I4</f>
+        <f>Hoja1!J4</f>
         <v>1059292</v>
       </c>
       <c r="C2" s="7">
-        <f>Hoja1!J4</f>
+        <f>Hoja1!K4</f>
         <v>897243</v>
       </c>
       <c r="D2" s="7">
-        <f>Hoja1!K4</f>
+        <f>Hoja1!L4</f>
         <v>909628</v>
       </c>
       <c r="E2" s="7">
-        <f>Hoja1!L4</f>
+        <f>Hoja1!M4</f>
         <v>1094317</v>
       </c>
       <c r="F2" s="7">
-        <f>Hoja1!M4</f>
+        <f>Hoja1!N4</f>
         <v>913346</v>
       </c>
       <c r="G2" s="7">
-        <f>Hoja1!N4</f>
+        <f>Hoja1!O4</f>
         <v>1086935</v>
       </c>
       <c r="H2" s="7">
-        <f>Hoja1!O4</f>
+        <f>Hoja1!P4</f>
         <v>902873</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="37.5" thickBot="1">
+      <c r="I2" s="7">
+        <f>Hoja1!Q4</f>
+        <v>899793</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="37.5" thickBot="1">
       <c r="A3" s="6" t="s">
         <v>13</v>
       </c>
       <c r="B3" s="7">
-        <f>Hoja1!I5</f>
+        <f>Hoja1!J5</f>
         <v>502504</v>
       </c>
       <c r="C3" s="7">
-        <f>Hoja1!J5</f>
+        <f>Hoja1!K5</f>
         <v>555463</v>
       </c>
       <c r="D3" s="7">
-        <f>Hoja1!K5</f>
+        <f>Hoja1!L5</f>
         <v>399181</v>
       </c>
       <c r="E3" s="7">
-        <f>Hoja1!L5</f>
+        <f>Hoja1!M5</f>
         <v>662813</v>
       </c>
       <c r="F3" s="7">
-        <f>Hoja1!M5</f>
+        <f>Hoja1!N5</f>
         <v>580264</v>
       </c>
       <c r="G3" s="7">
-        <f>Hoja1!N5</f>
+        <f>Hoja1!O5</f>
         <v>630050</v>
       </c>
       <c r="H3" s="7">
-        <f>Hoja1!O5</f>
+        <f>Hoja1!P5</f>
         <v>329766</v>
       </c>
-    </row>
-    <row r="4" spans="1:10" ht="25.5" thickBot="1">
+      <c r="I3" s="7">
+        <f>Hoja1!Q5</f>
+        <v>577910</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="25.5" thickBot="1">
       <c r="A4" s="6" t="s">
         <v>21</v>
       </c>
       <c r="B4" s="8">
-        <f>Hoja1!I6</f>
+        <f>Hoja1!J6</f>
         <v>0.47399999999999998</v>
       </c>
       <c r="C4" s="8">
-        <f>Hoja1!J6</f>
+        <f>Hoja1!K6</f>
         <v>0.61899999999999999</v>
       </c>
       <c r="D4" s="8">
-        <f>Hoja1!K6</f>
+        <f>Hoja1!L6</f>
         <v>0.439</v>
       </c>
       <c r="E4" s="8">
-        <f>Hoja1!L6</f>
+        <f>Hoja1!M6</f>
         <v>0.60599999999999998</v>
       </c>
       <c r="F4" s="8">
-        <f>Hoja1!M6</f>
+        <f>Hoja1!N6</f>
         <v>0.63500000000000001</v>
       </c>
       <c r="G4" s="8">
-        <f>Hoja1!N6</f>
+        <f>Hoja1!O6</f>
         <v>0.57999999999999996</v>
       </c>
       <c r="H4" s="8">
-        <f>Hoja1!O6</f>
+        <f>Hoja1!P6</f>
         <v>0.36499999999999999</v>
       </c>
-    </row>
-    <row r="5" spans="1:10" ht="15.75" thickBot="1">
+      <c r="I4" s="8">
+        <f>Hoja1!Q6</f>
+        <v>0.64200000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="15.75" thickBot="1">
       <c r="A5" s="6" t="s">
         <v>22</v>
       </c>
       <c r="B5" s="7">
-        <f>Hoja1!I7</f>
+        <f>Hoja1!J7</f>
         <v>9317</v>
       </c>
       <c r="C5" s="7">
-        <f>Hoja1!J7</f>
+        <f>Hoja1!K7</f>
         <v>30275</v>
       </c>
       <c r="D5" s="7">
-        <f>Hoja1!K7</f>
+        <f>Hoja1!L7</f>
         <v>58669</v>
       </c>
       <c r="E5" s="7">
-        <f>Hoja1!L7</f>
+        <f>Hoja1!M7</f>
         <v>104413</v>
       </c>
       <c r="F5" s="7">
-        <f>Hoja1!M7</f>
+        <f>Hoja1!N7</f>
         <v>140846</v>
       </c>
       <c r="G5" s="7">
-        <f>Hoja1!N7</f>
+        <f>Hoja1!O7</f>
         <v>133808</v>
       </c>
       <c r="H5" s="7">
-        <f>Hoja1!O7</f>
+        <f>Hoja1!P7</f>
         <v>103151</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="25.5" thickBot="1">
+      <c r="I5" s="7">
+        <f>Hoja1!Q7</f>
+        <v>176491</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="25.5" thickBot="1">
       <c r="A6" s="6" t="s">
         <v>30</v>
       </c>
       <c r="B6" s="7">
-        <f>Hoja1!I8</f>
+        <f>Hoja1!J8</f>
         <v>9287</v>
       </c>
       <c r="C6" s="7">
-        <f>Hoja1!J8</f>
+        <f>Hoja1!K8</f>
         <v>30243</v>
       </c>
       <c r="D6" s="7">
-        <f>Hoja1!K8</f>
+        <f>Hoja1!L8</f>
         <v>58614</v>
       </c>
       <c r="E6" s="7">
-        <f>Hoja1!L8</f>
+        <f>Hoja1!M8</f>
         <v>104313</v>
       </c>
       <c r="F6" s="7">
-        <f>Hoja1!M8</f>
+        <f>Hoja1!N8</f>
         <v>140764</v>
       </c>
       <c r="G6" s="7">
-        <f>Hoja1!N8</f>
+        <f>Hoja1!O8</f>
         <v>133662</v>
       </c>
       <c r="H6" s="7">
-        <f>Hoja1!O8</f>
+        <f>Hoja1!P8</f>
         <v>103105</v>
       </c>
-    </row>
-    <row r="7" spans="1:10" ht="24.75">
+      <c r="I6" s="7">
+        <f>Hoja1!Q8</f>
+        <v>176329</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="24.75">
       <c r="A7" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="B7" s="33">
-        <f>Hoja1!I9</f>
+      <c r="B7" s="32">
+        <f>Hoja1!J9</f>
         <v>30</v>
       </c>
-      <c r="C7" s="33">
-        <f>Hoja1!J9</f>
+      <c r="C7" s="32">
+        <f>Hoja1!K9</f>
         <v>32</v>
       </c>
-      <c r="D7" s="33">
-        <f>Hoja1!K9</f>
+      <c r="D7" s="32">
+        <f>Hoja1!L9</f>
         <v>55</v>
       </c>
-      <c r="E7" s="33">
-        <f>Hoja1!L9</f>
+      <c r="E7" s="32">
+        <f>Hoja1!M9</f>
         <v>100</v>
       </c>
-      <c r="F7" s="33">
-        <f>Hoja1!M9</f>
+      <c r="F7" s="32">
+        <f>Hoja1!N9</f>
         <v>82</v>
       </c>
-      <c r="G7" s="33">
-        <f>Hoja1!N9</f>
+      <c r="G7" s="32">
+        <f>Hoja1!O9</f>
         <v>146</v>
       </c>
-      <c r="H7" s="33">
-        <f>Hoja1!O9</f>
+      <c r="H7" s="32">
+        <f>Hoja1!P9</f>
         <v>46</v>
       </c>
-    </row>
-    <row r="8" spans="1:10" ht="37.5" thickBot="1">
+      <c r="I7" s="32">
+        <f>Hoja1!Q9</f>
+        <v>162</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="37.5" thickBot="1">
       <c r="A8" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="B8" s="34"/>
-      <c r="C8" s="34"/>
-      <c r="D8" s="34"/>
-      <c r="E8" s="34"/>
-      <c r="F8" s="34"/>
-      <c r="G8" s="34"/>
-      <c r="H8" s="34"/>
-    </row>
-    <row r="9" spans="1:10" ht="61.5" thickBot="1">
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
+    </row>
+    <row r="9" spans="1:11" ht="61.5" thickBot="1">
       <c r="A9" s="6" t="s">
         <v>41</v>
       </c>
       <c r="B9" s="7" t="e">
-        <f>Hoja1!I11</f>
+        <f>Hoja1!J11</f>
         <v>#VALUE!</v>
       </c>
       <c r="C9" s="7" t="e">
-        <f>Hoja1!J11</f>
+        <f>Hoja1!K11</f>
         <v>#VALUE!</v>
       </c>
       <c r="D9" s="7" t="e">
-        <f>Hoja1!K11</f>
+        <f>Hoja1!L11</f>
         <v>#VALUE!</v>
       </c>
       <c r="E9" s="7" t="e">
-        <f>Hoja1!L11</f>
+        <f>Hoja1!M11</f>
         <v>#VALUE!</v>
       </c>
       <c r="F9" s="7" t="e">
-        <f>Hoja1!M11</f>
+        <f>Hoja1!N11</f>
         <v>#VALUE!</v>
       </c>
       <c r="G9" s="7">
-        <f>Hoja1!N11</f>
+        <f>Hoja1!O11</f>
         <v>1</v>
       </c>
       <c r="H9" s="7" t="e">
-        <f>Hoja1!O11</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" ht="49.5" thickBot="1">
+        <f>Hoja1!P11</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I9" s="7">
+        <f>Hoja1!Q11</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="49.5" thickBot="1">
       <c r="A10" s="6" t="s">
         <v>44</v>
       </c>
       <c r="B10" s="7">
-        <f>Hoja1!I12</f>
+        <f>Hoja1!J12</f>
         <v>364</v>
       </c>
       <c r="C10" s="7">
-        <f>Hoja1!J12</f>
+        <f>Hoja1!K12</f>
         <v>789</v>
       </c>
       <c r="D10" s="7">
-        <f>Hoja1!K12</f>
+        <f>Hoja1!L12</f>
         <v>910</v>
       </c>
       <c r="E10" s="7">
-        <f>Hoja1!L12</f>
+        <f>Hoja1!M12</f>
         <v>2373</v>
       </c>
       <c r="F10" s="7">
-        <f>Hoja1!M12</f>
+        <f>Hoja1!N12</f>
         <v>4384</v>
       </c>
       <c r="G10" s="7">
-        <f>Hoja1!N12</f>
+        <f>Hoja1!O12</f>
         <v>3045</v>
       </c>
       <c r="H10" s="7">
-        <f>Hoja1!O12</f>
+        <f>Hoja1!P12</f>
         <v>2019</v>
       </c>
-    </row>
-    <row r="11" spans="1:10" ht="49.5" thickBot="1">
+      <c r="I10" s="7">
+        <f>Hoja1!Q12</f>
+        <v>4593</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="49.5" thickBot="1">
       <c r="A11" s="6" t="s">
         <v>49</v>
       </c>
-      <c r="B11" s="7">
-        <f>Hoja1!I13</f>
+      <c r="B11" s="8">
+        <f>Hoja1!J13</f>
         <v>8.9999999999999993E-3</v>
       </c>
-      <c r="C11" s="7">
-        <f>Hoja1!J13</f>
+      <c r="C11" s="8">
+        <f>Hoja1!K13</f>
         <v>3.4000000000000002E-2</v>
       </c>
-      <c r="D11" s="7">
-        <f>Hoja1!K13</f>
+      <c r="D11" s="8">
+        <f>Hoja1!L13</f>
         <v>6.5000000000000002E-2</v>
       </c>
-      <c r="E11" s="7">
-        <f>Hoja1!L13</f>
+      <c r="E11" s="8">
+        <f>Hoja1!M13</f>
         <v>9.5000000000000001E-2</v>
       </c>
-      <c r="F11" s="7">
-        <f>Hoja1!M13</f>
+      <c r="F11" s="8">
+        <f>Hoja1!N13</f>
         <v>0.154</v>
       </c>
-      <c r="G11" s="7">
-        <f>Hoja1!N13</f>
+      <c r="G11" s="8">
+        <f>Hoja1!O13</f>
         <v>0.123</v>
       </c>
-      <c r="H11" s="7">
-        <f>Hoja1!O13</f>
+      <c r="H11" s="8">
+        <f>Hoja1!P13</f>
         <v>0.114</v>
       </c>
-    </row>
-    <row r="12" spans="1:10" ht="49.5" thickBot="1">
+      <c r="I11" s="8">
+        <f>Hoja1!Q13</f>
+        <v>0.19600000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" ht="49.5" thickBot="1">
       <c r="A12" s="6" t="s">
         <v>51</v>
       </c>
       <c r="B12" s="13">
-        <f>Hoja1!I14</f>
+        <f>Hoja1!J14</f>
         <v>1.9E-2</v>
       </c>
       <c r="C12" s="13">
-        <f>Hoja1!J14</f>
+        <f>Hoja1!K14</f>
         <v>5.5E-2</v>
       </c>
       <c r="D12" s="13">
-        <f>Hoja1!K14</f>
+        <f>Hoja1!L14</f>
         <v>0.14699999999999999</v>
       </c>
       <c r="E12" s="13">
-        <f>Hoja1!L14</f>
+        <f>Hoja1!M14</f>
         <v>0.158</v>
       </c>
       <c r="F12" s="13">
-        <f>Hoja1!M14</f>
+        <f>Hoja1!N14</f>
         <v>0.24299999999999999</v>
       </c>
       <c r="G12" s="13">
-        <f>Hoja1!N14</f>
+        <f>Hoja1!O14</f>
         <v>0.21199999999999999</v>
       </c>
       <c r="H12" s="13">
-        <f>Hoja1!O14</f>
+        <f>Hoja1!P14</f>
         <v>0.313</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="49.5" thickBot="1">
+      <c r="I12" s="13">
+        <f>Hoja1!Q14</f>
+        <v>0.30499999999999999</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" ht="49.5" thickBot="1">
       <c r="A13" s="6" t="s">
         <v>52</v>
       </c>
-      <c r="B13" s="7">
-        <f>Hoja1!I15</f>
-        <v>7.1999999999999993</v>
-      </c>
-      <c r="C13" s="7">
+      <c r="B13" s="8">
         <f>Hoja1!J15</f>
-        <v>17.599999999999998</v>
-      </c>
-      <c r="D13" s="7">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="C13" s="8">
         <f>Hoja1!K15</f>
-        <v>45.4</v>
-      </c>
-      <c r="E13" s="7">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="D13" s="8">
         <f>Hoja1!L15</f>
-        <v>44</v>
-      </c>
-      <c r="F13" s="7">
+        <v>0.45400000000000001</v>
+      </c>
+      <c r="E13" s="8">
         <f>Hoja1!M15</f>
-        <v>56.399999999999991</v>
-      </c>
-      <c r="G13" s="7" t="e">
+        <v>0.44</v>
+      </c>
+      <c r="F13" s="8">
         <f>Hoja1!N15</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="H13" s="7">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="G13" s="8" t="e">
         <f>Hoja1!O15</f>
-        <v>59.199999999999996</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10">
-      <c r="A14" s="37" t="s">
+        <v>#VALUE!</v>
+      </c>
+      <c r="H13" s="8">
+        <f>Hoja1!P15</f>
+        <v>0.59199999999999997</v>
+      </c>
+      <c r="I13" s="8">
+        <f>Hoja1!Q15</f>
+        <v>0.59599999999999997</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11">
+      <c r="A14" s="30" t="s">
         <v>54</v>
       </c>
-      <c r="B14" s="33" t="e">
-        <f>Hoja1!I16</f>
-        <v>#VALUE!</v>
-      </c>
-      <c r="C14" s="33" t="e">
+      <c r="B14" s="32" t="e">
         <f>Hoja1!J16</f>
         <v>#VALUE!</v>
       </c>
-      <c r="D14" s="33" t="e">
+      <c r="C14" s="32" t="e">
         <f>Hoja1!K16</f>
         <v>#VALUE!</v>
       </c>
-      <c r="E14" s="33" t="e">
+      <c r="D14" s="32" t="e">
         <f>Hoja1!L16</f>
         <v>#VALUE!</v>
       </c>
-      <c r="F14" s="33">
+      <c r="E14" s="32" t="e">
         <f>Hoja1!M16</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="F14" s="32">
+        <f>Hoja1!N16</f>
         <v>3.9</v>
       </c>
-      <c r="G14" s="33">
-        <f>Hoja1!N16</f>
+      <c r="G14" s="32">
+        <f>Hoja1!O16</f>
         <v>4.2</v>
       </c>
-      <c r="H14" s="33">
-        <f>Hoja1!O16</f>
+      <c r="H14" s="32">
+        <f>Hoja1!P16</f>
         <v>4.6899999999999995</v>
       </c>
-    </row>
-    <row r="15" spans="1:10" ht="15.75" thickBot="1">
-      <c r="A15" s="38"/>
-      <c r="B15" s="34"/>
-      <c r="C15" s="34"/>
-      <c r="D15" s="34"/>
-      <c r="E15" s="34"/>
-      <c r="F15" s="34"/>
-      <c r="G15" s="34"/>
-      <c r="H15" s="34"/>
-    </row>
-    <row r="16" spans="1:10" ht="25.5" thickBot="1">
+      <c r="I14" s="32">
+        <f>Hoja1!Q16</f>
+        <v>5.71</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" ht="15.75" thickBot="1">
+      <c r="A15" s="31"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
+    </row>
+    <row r="16" spans="1:11" ht="25.5" thickBot="1">
       <c r="A16" s="6" t="s">
         <v>64</v>
       </c>
       <c r="B16" s="7" t="e">
-        <f>Hoja1!I18</f>
+        <f>Hoja1!J18</f>
         <v>#VALUE!</v>
       </c>
       <c r="C16" s="7" t="e">
-        <f>Hoja1!J18</f>
+        <f>Hoja1!K18</f>
         <v>#VALUE!</v>
       </c>
       <c r="D16" s="7" t="e">
-        <f>Hoja1!K18</f>
+        <f>Hoja1!L18</f>
         <v>#VALUE!</v>
       </c>
       <c r="E16" s="7" t="e">
-        <f>Hoja1!L18</f>
+        <f>Hoja1!M18</f>
         <v>#VALUE!</v>
       </c>
       <c r="F16" s="7" t="e">
-        <f>Hoja1!M18</f>
+        <f>Hoja1!N18</f>
         <v>#VALUE!</v>
       </c>
       <c r="G16" s="7" t="e">
-        <f>Hoja1!N18</f>
+        <f>Hoja1!O18</f>
         <v>#VALUE!</v>
       </c>
       <c r="H16" s="7" t="e">
-        <f>Hoja1!O18</f>
-        <v>#VALUE!</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" ht="37.5" thickBot="1">
+        <f>Hoja1!P18</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="I16" s="7" t="e">
+        <f>Hoja1!Q18</f>
+        <v>#VALUE!</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="37.5" thickBot="1">
       <c r="A17" s="6" t="s">
         <v>68</v>
       </c>
       <c r="B17" s="7" t="e">
-        <f>Hoja1!I19</f>
+        <f>Hoja1!J19</f>
         <v>#VALUE!</v>
       </c>
       <c r="C17" s="7" t="e">
-        <f>Hoja1!J19</f>
+        <f>Hoja1!K19</f>
         <v>#VALUE!</v>
       </c>
       <c r="D17" s="7" t="e">
-        <f>Hoja1!K19</f>
+        <f>Hoja1!L19</f>
         <v>#VALUE!</v>
       </c>
       <c r="E17" s="7" t="e">
-        <f>Hoja1!L19</f>
+        <f>Hoja1!M19</f>
         <v>#VALUE!</v>
       </c>
       <c r="F17" s="7">
-        <f>Hoja1!M19</f>
+        <f>Hoja1!N19</f>
         <v>2690</v>
       </c>
       <c r="G17" s="7">
-        <f>Hoja1!N19</f>
+        <f>Hoja1!O19</f>
         <v>11753</v>
       </c>
       <c r="H17" s="7">
-        <f>Hoja1!O19</f>
+        <f>Hoja1!P19</f>
         <v>11609</v>
       </c>
-    </row>
-    <row r="18" spans="1:8" ht="49.5" thickBot="1">
+      <c r="I17" s="7">
+        <f>Hoja1!Q19</f>
+        <v>22084</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="49.5" thickBot="1">
       <c r="A18" s="6" t="s">
         <v>72</v>
       </c>
       <c r="B18" s="7" t="e">
-        <f>Hoja1!I20</f>
+        <f>Hoja1!J20</f>
         <v>#VALUE!</v>
       </c>
       <c r="C18" s="7" t="e">
-        <f>Hoja1!J20</f>
+        <f>Hoja1!K20</f>
         <v>#VALUE!</v>
       </c>
       <c r="D18" s="7" t="e">
-        <f>Hoja1!K20</f>
+        <f>Hoja1!L20</f>
         <v>#VALUE!</v>
       </c>
       <c r="E18" s="7" t="e">
-        <f>Hoja1!L20</f>
+        <f>Hoja1!M20</f>
         <v>#VALUE!</v>
       </c>
       <c r="F18" s="7">
-        <f>Hoja1!M20</f>
+        <f>Hoja1!N20</f>
         <v>1.9</v>
       </c>
       <c r="G18" s="7">
-        <f>Hoja1!N20</f>
+        <f>Hoja1!O20</f>
         <v>8.6</v>
       </c>
       <c r="H18" s="7">
-        <f>Hoja1!O20</f>
+        <f>Hoja1!P20</f>
         <v>11</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" ht="61.5" thickBot="1">
+      <c r="I18" s="7">
+        <f>Hoja1!Q20</f>
+        <v>12.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="61.5" thickBot="1">
       <c r="A19" s="23" t="s">
         <v>73</v>
       </c>
       <c r="B19" s="7" t="e">
-        <f>Hoja1!I21</f>
+        <f>Hoja1!J21</f>
         <v>#VALUE!</v>
       </c>
       <c r="C19" s="7" t="e">
-        <f>Hoja1!J21</f>
+        <f>Hoja1!K21</f>
         <v>#VALUE!</v>
       </c>
       <c r="D19" s="7" t="e">
-        <f>Hoja1!K21</f>
+        <f>Hoja1!L21</f>
         <v>#VALUE!</v>
       </c>
       <c r="E19" s="7" t="e">
-        <f>Hoja1!L21</f>
+        <f>Hoja1!M21</f>
         <v>#VALUE!</v>
       </c>
       <c r="F19" s="7" t="e">
-        <f>Hoja1!M21</f>
+        <f>Hoja1!N21</f>
         <v>#VALUE!</v>
       </c>
       <c r="G19" s="7">
-        <f>Hoja1!N21</f>
+        <f>Hoja1!O21</f>
         <v>3.4000000000000004</v>
       </c>
       <c r="H19" s="7">
-        <f>Hoja1!O21</f>
+        <f>Hoja1!P21</f>
         <v>4</v>
       </c>
+      <c r="I19" s="7">
+        <f>Hoja1!Q21</f>
+        <v>4.3</v>
+      </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="17">
+    <mergeCell ref="G7:G8"/>
+    <mergeCell ref="H7:H8"/>
+    <mergeCell ref="I7:I8"/>
+    <mergeCell ref="I14:I15"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
     <mergeCell ref="F14:F15"/>
     <mergeCell ref="G14:G15"/>
     <mergeCell ref="H14:H15"/>
@@ -3101,13 +3347,6 @@
     <mergeCell ref="C14:C15"/>
     <mergeCell ref="D14:D15"/>
     <mergeCell ref="E14:E15"/>
-    <mergeCell ref="B7:B8"/>
-    <mergeCell ref="C7:C8"/>
-    <mergeCell ref="D7:D8"/>
-    <mergeCell ref="E7:E8"/>
-    <mergeCell ref="F7:F8"/>
-    <mergeCell ref="G7:G8"/>
-    <mergeCell ref="H7:H8"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Añado Gráficos de estonia Cambio un gráfico hecho a mano por otro hecho en Cacoo. Comento literatura que no debe salir el en documento final
</commit_message>
<xml_diff>
--- a/doc/memoria/recursos/estonia.xlsx
+++ b/doc/memoria/recursos/estonia.xlsx
@@ -1024,11 +1024,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="133998848"/>
-        <c:axId val="183520256"/>
+        <c:axId val="49040000"/>
+        <c:axId val="49045888"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="133998848"/>
+        <c:axId val="49040000"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1037,7 +1037,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="183520256"/>
+        <c:crossAx val="49045888"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1045,18 +1045,28 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="183520256"/>
+        <c:axId val="49045888"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="#,##0" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="133998848"/>
+        <c:crossAx val="49040000"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1092,11 +1102,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -1196,11 +1202,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="144485376"/>
-        <c:axId val="144499456"/>
+        <c:axId val="49078272"/>
+        <c:axId val="49079808"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="144485376"/>
+        <c:axId val="49078272"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1209,7 +1215,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144499456"/>
+        <c:crossAx val="49079808"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1217,24 +1223,34 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="144499456"/>
+        <c:axId val="49079808"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="144485376"/>
+        <c:crossAx val="49078272"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="r"/>
+      <c:legendPos val="b"/>
       <c:layout/>
       <c:overlay val="0"/>
     </c:legend>
@@ -1497,11 +1513,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="193542016"/>
-        <c:axId val="193543552"/>
+        <c:axId val="50215936"/>
+        <c:axId val="50230016"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="193542016"/>
+        <c:axId val="50215936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1510,7 +1526,7 @@
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193543552"/>
+        <c:crossAx val="50230016"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1518,18 +1534,29 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="193543552"/>
+        <c:axId val="50230016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="1"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="0.00%" sourceLinked="1"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln>
+              <a:solidFill>
+                <a:schemeClr val="accent1">
+                  <a:alpha val="40000"/>
+                </a:schemeClr>
+              </a:solidFill>
+            </a:ln>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="0%" sourceLinked="0"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="193542016"/>
+        <c:crossAx val="50215936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1555,14 +1582,14 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>209550</xdr:colOff>
       <xdr:row>2</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
+      <xdr:col>24</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
       <xdr:row>9</xdr:row>
       <xdr:rowOff>428625</xdr:rowOff>
     </xdr:to>
@@ -1586,15 +1613,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>552450</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>685800</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>47625</xdr:rowOff>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>142875</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -1615,16 +1642,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>2</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>219074</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>114299</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>476250</xdr:rowOff>
+      <xdr:rowOff>371475</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3110,8 +3137,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="V12" sqref="V12"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="T11" sqref="T11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3796,11 +3823,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="A15:A16"/>
-    <mergeCell ref="B15:B16"/>
-    <mergeCell ref="C15:C16"/>
-    <mergeCell ref="D15:D16"/>
-    <mergeCell ref="E15:E16"/>
     <mergeCell ref="G8:G9"/>
     <mergeCell ref="H8:H9"/>
     <mergeCell ref="I8:I9"/>
@@ -3813,6 +3835,11 @@
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="G15:G16"/>
     <mergeCell ref="H15:H16"/>
+    <mergeCell ref="A15:A16"/>
+    <mergeCell ref="B15:B16"/>
+    <mergeCell ref="C15:C16"/>
+    <mergeCell ref="D15:D16"/>
+    <mergeCell ref="E15:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>